<commit_message>
Updated tests to prevent os dependent test noise
Detail: https://github.com/dotnet/runtime/issues/108742
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/Misc/CellValues.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/Misc/CellValues.xlsx
@@ -35,7 +35,7 @@
     <x:t>GetFormattedString()</x:t>
   </x:si>
   <x:si>
-    <x:t>9/2/2010 12:00:00 AM</x:t>
+    <x:t>09/02/2010 00:00:00</x:t>
   </x:si>
   <x:si>
     <x:t>2010-Sep-02</x:t>
@@ -478,7 +478,7 @@
     <x:col min="3" max="3" width="10.855466" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="13.930125" style="0" customWidth="1"/>
     <x:col min="5" max="5" width="20.049541" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="21.936327" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="20.598129" style="0" customWidth="1"/>
     <x:col min="7" max="7" width="20.875341" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>

</xml_diff>